<commit_message>
job detail parsing working correctly
</commit_message>
<xml_diff>
--- a/job_listings.xlsx
+++ b/job_listings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>date_posted</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>url</t>
         </is>
       </c>
@@ -474,251 +469,965 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>https://boards.greenhouse.io/waymo/jobs/5853062</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Celonis</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Software Engineer - Machine Learning</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Palo Alto, US, California</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/vannevarlabs/jobs/4366534007?gh_src=5d6535b17us</t>
+          <t>https://boards.greenhouse.io/celonis/jobs/5814476003</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pinterest Job Advertisements</t>
+          <t>The Allen Institute for AI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer II</t>
+          <t>Machine Learning Engineer, AllenNLP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>San Francisco, CA, US; Remote, US</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/pinterestjobadvertisements/jobs/5951216</t>
+          <t>https://boards.greenhouse.io/thealleninstitute/jobs/5801474</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Formation Bio</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Software Engineer, Emerging Products (AI/LLM)</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>New York, NY</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/formationbio/jobs/5947901</t>
+          <t>https://boards.greenhouse.io/vannevarlabs/jobs/43665340075653517</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ada</t>
+          <t>Truveta</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Machine Learning Scientist</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Remote Canada or Remote Israel</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/ada18/jobs/4368229007</t>
+          <t>https://boards.greenhouse.io/truveta/jobs/5028154004</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Spotter</t>
+          <t>Profluent</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AI Prompt Engineer</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Culver City, California, United States</t>
+          <t>Berkeley, California, United States</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/spotter/jobs/4417247005</t>
+          <t>https://boards.greenhouse.io/profluent/jobs/4000661008</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Analytics Engineer</t>
+          <t>NewsBreak</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Machine Learning Engineer (Junior &amp; New Grad)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Bellevue, Washington, United States</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/octoenergy/442fe0f4-cbc7-4942-a004-5ca84ce950e8</t>
+          <t>https://boards.greenhouse.io/newsbreak/jobs/4338876006</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Smartling</t>
+          <t>Pinterest Job Advertisements</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Linguistic Engineer</t>
+          <t>Machine Learning Engineer II</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>San Francisco, CA, US; Remote, US</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/smartling/jobs/5950645?utm_source=Felicis+Ventures+job+board&amp;utm_medium=getro.com&amp;gh_src=Felicis+Ventures+job+board</t>
+          <t>https://boards.greenhouse.io/pinterestjobadvertisements/jobs/5951216</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vonage</t>
+          <t>CoVar</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Backend Engineer</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bangalore</t>
+          <t>Durham, NC</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/vonage/jobs/7333871002?gh_src=Blind</t>
+          <t>https://boards.greenhouse.io/covar/jobs/4021592007</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EBANX</t>
+          <t>Notion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mid-level Software Engineer</t>
+          <t>Software Engineer, Search</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>New York, New York</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/ebanx/jobs/5971275003</t>
+          <t>https://boards.greenhouse.io/notion/jobs/5650399003</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/latitude/jobs/5574737</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kitware</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Clifton Park, New York / Arlington, Virginia / Dayton, OH-Customer Site / Minneapolis, MN / Rome, NY-Customer Site / Santa Fe, New Mexico / Carrboro, North Carolina</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/kitware/68e131bd-89fc-4866-8305-1bd64bae5ef8</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Scale AI</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer, Federal</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>San Francisco, CA; New York, NY; Washington, DC</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/scaleai/jobs/4281519005</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/allturtles/jobs/7078885002557951</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Formation Bio</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Software Engineer, Emerging Products (AI/LLM)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>New York, NY</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/formationbio/jobs/5947901</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Latitude AI</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Software Engineer II, Software Factory</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Pittsburgh PA, Hybrid, Remote</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/latitude/jobs/5938440</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/spacex/jobs/73373760027337376002</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Re:Build Manufacturing</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer for Advanced Manufacturing Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Framingham, MA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/rebuildmanufacturing/jobs/4334609005</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ada</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Machine Learning Scientist</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Remote Canada or Remote Israel</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/ada18/jobs/4368229007</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Scythe Robotics</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Cognition Robot Software Engineer</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Remote, US</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/scytherobotics/jobs/4362218006</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Spotter</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AI Prompt Engineer</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Culver City, California, United States</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/spotter/jobs/4417247005</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>San Francisco, California</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/wandb/105546b7-492f-42a8-a149-407105dbffe7</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/captivation/jobs/400605000871798</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Piaggio Fast Forward</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Robotics and AI Engineering Co-Op</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Boston, Massachusetts, United States</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/piaggiofastforward/jobs/5904398</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Cognite</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Machine Learning Engineer – LLM &amp; Generative AI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Austin, Texas</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/cognite/41c1077b-5276-4503-83ac-9fe1e652eb80</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/tripadvisor/jobs/5673849</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Enterra Solutions</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Data Engineer</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/enterrasolutions/jobs/4040011007</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>GitLab</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Backend Engineer, MLOps</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/gitlab/jobs/7296739002</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Seldon</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Software Engineer - Golang (India - Remote)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/seldon/jobs/5970423003</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Kitware</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Natural Language Processing (NLP) Researcher</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Clifton Park, New York</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/kitware/12290434-b677-4911-8b81-2157e582621f</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Accenture Federal Services</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ML &amp; Data Ops</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Washington, DC</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/accenturefederalservices/jobs/4279211006</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>RippleMatch Opportunities</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>HRL Laboratories - Generative AI Navigation Intern, application via RippleMatch</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Malibu, CA</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/ripplematchinterns/jobs/7417813002</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Truveta</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ML Postdoc Researcher - LLMs &amp; Generative AI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Seattle, WA</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/truveta/jobs/4898482004</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Box</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Software Engineer, Observability</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Redwood City, CA</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/boxinc/jobs/5614752</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://boards.eu.greenhouse.io/abbyy/jobs/4302613101</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Vonage</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Python - Backend Engineer</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/vonage/jobs/7090195002</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/spacex/jobs/72336960027233696002</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Together AI</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>AI Researcher, NLP and Computer Vision</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/togetherai/jobs/4188035007</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Isomorphic Labs</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Bioinformatics Engineer</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/isomorphiclabs/jobs/5035792004</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Smartling</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Linguistic Engineer</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/smartling/jobs/5950645</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>KoBold Metals</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Infrastructure Engineer</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Remote</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/koboldmetals/jobs/4400868005</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Latitude AI</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Software Engineer II, Cloud Services</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Palo Alto CA, Pittsburgh PA, Detroit MI</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/latitude/jobs/5848856</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>InstaDeep</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Research Engineer</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://jobs.eu.lever.co/instadeep/dfd57254-147a-40e3-b6fb-efbc557d64a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Cars Commerce</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Data Scientist II</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>United States, Remote</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/carsdotcom/jobs/5808218</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Fama Technologies Inc.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Junior Machine Learning Engineer</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Los Angeles, CA</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/fama/90a571a3-1cef-4f6b-9ce4-c5c63e8e1604</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Bolster Inc.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Front-End Engineer</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Noida</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/bolster/f05cab87-0afb-4208-afdc-d6ede35b781e</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
in us location not working yet
</commit_message>
<xml_diff>
--- a/job_listings.xlsx
+++ b/job_listings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>in_us</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>url</t>
         </is>
       </c>
@@ -467,53 +472,54 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>https://boards.greenhouse.io/waymo/jobs/5853062</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Celonis</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Software Engineer - Machine Learning</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Palo Alto, US, California</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/celonis/jobs/5814476003</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/waymo/jobs/5927862</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>The Allen Institute for AI</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer, AllenNLP</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/thealleninstitute/jobs/5801474</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://support.greenhouse.io/hc/en-us/</t>
         </is>
       </c>
     </row>
@@ -529,141 +535,150 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/vannevarlabs/jobs/43665340075653517</t>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/stripe/jobs/5677295</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Truveta</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/truveta/jobs/5028154004</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/waymo/jobs/5853040</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Profluent</t>
+          <t>NPR</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>Elections Graphics Reporter - Temporary</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Berkeley, California, United States</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/profluent/jobs/4000661008</t>
+          <t>Washington, District of Columbia, United States</t>
+        </is>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/nationalpublicradioinc/jobs/4414927005</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NewsBreak</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer (Junior &amp; New Grad)</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bellevue, Washington, United States</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/newsbreak/jobs/4338876006</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/shopltk/jobs/5972036003852913</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pinterest Job Advertisements</t>
+          <t>NPR</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer II</t>
+          <t>Producer 3, All Things Considered</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>San Francisco, CA, US; Remote, US</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/pinterestjobadvertisements/jobs/5951216</t>
+          <t>Washington, District of Columbia, United States</t>
+        </is>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/nationalpublicradioinc/jobs/4415681005</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>CoVar</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Durham, NC</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/covar/jobs/4021592007</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/outlier/jobs/440817500539905</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Notion</t>
+          <t>Intercom</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Software Engineer, Search</t>
+          <t>Recruiting Coordinator (12 Month Contract)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>New York, New York</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/notion/jobs/5650399003</t>
+          <t>Dublin, Ireland</t>
+        </is>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/intercom/jobs/5952537</t>
         </is>
       </c>
     </row>
@@ -679,53 +694,58 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/latitude/jobs/5574737</t>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/hs/jobs/55238762020202020</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Kitware</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Clifton Park, New York / Arlington, Virginia / Dayton, OH-Customer Site / Minneapolis, MN / Rome, NY-Customer Site / Santa Fe, New Mexico / Carrboro, North Carolina</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/kitware/68e131bd-89fc-4866-8305-1bd64bae5ef8</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/porchcom/jobs/7287023002</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Scale AI</t>
+          <t>Intercom</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer, Federal</t>
+          <t>Sales Development Representative</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>San Francisco, CA; New York, NY; Washington, DC</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/scaleai/jobs/4281519005</t>
+          <t>Chicago, Illinois</t>
+        </is>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/intercom/jobs/5948718</t>
         </is>
       </c>
     </row>
@@ -741,181 +761,212 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/allturtles/jobs/7078885002557951</t>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/waymark/jobs/41034650052020</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Formation Bio</t>
+          <t>NPR</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Software Engineer, Emerging Products (AI/LLM)</t>
+          <t>Editor II, Up First, Morning Edition - Temporary</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>New York, NY</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/formationbio/jobs/5947901</t>
+          <t>Washington, District of Columbia, United States</t>
+        </is>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/nationalpublicradioinc/jobs/4415069005</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Latitude AI</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Software Engineer II, Software Factory</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Pittsburgh PA, Hybrid, Remote</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/latitude/jobs/5938440</t>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/appen/7ed5786e-47dd-4af6-91f1-622b243f1b6d</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>The Scion Group</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Leasing Consultant</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/spacex/jobs/73373760027337376002</t>
+          <t>West Edge, Colorado Springs, Colorado, Untied States</t>
+        </is>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/thesciongroupllc/jobs/7440728002</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Re:Build Manufacturing</t>
+          <t>ZipRecruiter</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer for Advanced Manufacturing Artificial Intelligence</t>
+          <t>Director of Payroll</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Framingham, MA</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/rebuildmanufacturing/jobs/4334609005</t>
+          <t>Santa Monica, CA</t>
+        </is>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/ziprecruiter/jobs/5948915</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ada</t>
+          <t>Relogistics Services</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Machine Learning Scientist</t>
+          <t>Forklift Operator</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Remote Canada or Remote Israel</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/ada18/jobs/4368229007</t>
+          <t>Olney, Illinois, United States</t>
+        </is>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/relogistics/jobs/4416863005</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Scythe Robotics</t>
+          <t>Samsung Semiconductor</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cognition Robot Software Engineer</t>
+          <t>Financial Operations Specialist (Contractor)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Remote, US</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/scytherobotics/jobs/4362218006</t>
+          <t>San Jose, California, United States</t>
+        </is>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/samsungsemiconductor/jobs/5979110003</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Spotter</t>
+          <t>Digimarc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AI Prompt Engineer</t>
+          <t>Customer Success Director (Remote, US CST/EST only)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Culver City, California, United States</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/spotter/jobs/4417247005</t>
+          <t>Atlanta, GA / Boston, MA / Chicago, IL / Miami, FL / New York, NY / Remote</t>
+        </is>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/digimarc/ae781209-2894-4bb0-86e7-ff43f1211a2f</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Revolution Space</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Director of Engineering</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>San Francisco, California</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/wandb/105546b7-492f-42a8-a149-407105dbffe7</t>
+          <t>U.S Locations / Greenbelt, MD / DC Metro Area / Boston, MA</t>
+        </is>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/revolutionspace/0043110e-633f-41cb-bd88-6cc133aee2db</t>
         </is>
       </c>
     </row>
@@ -931,252 +982,296 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/captivation/jobs/400605000871798</t>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://boards.greenhouse.io/samsungsemiconductor/jobs/59791510031272653</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Piaggio Fast Forward</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Robotics and AI Engineering Co-Op</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Boston, Massachusetts, United States</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/piaggiofastforward/jobs/5904398</t>
+          <t>Milford, OH - Option Care (cust site)</t>
+        </is>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/gouspack/41a6bfef-3850-436f-a25f-7ecdc535a492</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cognite</t>
+          <t>Foodsmart</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer – LLM &amp; Generative AI</t>
+          <t>People Operations Analyst</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Austin, Texas</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/cognite/41c1077b-5276-4503-83ac-9fe1e652eb80</t>
+          <t>Remote (US)</t>
+        </is>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/foodsmart/1a3df7bb-5bd8-47f0-985e-a795e55c4cfa</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Productiv</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Head of Sales</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/tripadvisor/jobs/5673849</t>
+          <t>Palo Alto, CA / Remote, USA</t>
+        </is>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/productiv/135b8d4f-ee0b-4468-831c-d5eafeef7bb0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Enterra Solutions</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Remote</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/enterrasolutions/jobs/4040011007</t>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/welocalize/cf3a303c-c2ee-4344-b3a8-3f0e495c082f</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Backend Engineer, MLOps</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Remote</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/gitlab/jobs/7296739002</t>
+          <t>Philippines / Remote</t>
+        </is>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/loadsmart/f739cb61-5df6-4a5e-a911-e1cf604d12ac</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Seldon</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Software Engineer - Golang (India - Remote)</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/seldon/jobs/5970423003</t>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/welocalize/cf3a303c-c2ee-4344-b3a8-3f0e495c082f</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kitware</t>
+          <t>High Tech High</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Natural Language Processing (NLP) Researcher</t>
+          <t>US History Teacher</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Clifton Park, New York</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/kitware/12290434-b677-4911-8b81-2157e582621f</t>
+          <t>Point Loma, California</t>
+        </is>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/hightechhigh/63062cba-8213-4fda-afb6-df8de1cc7660</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Accenture Federal Services</t>
+          <t>Thrasio</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ML &amp; Data Ops</t>
+          <t>Director, Quality Assurance and Product Integrity</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/accenturefederalservices/jobs/4279211006</t>
+          <t>United States (Remote)</t>
+        </is>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/thrasio/a25c5291-ac69-407f-93cf-a434ee49fddf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>RippleMatch Opportunities</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>HRL Laboratories - Generative AI Navigation Intern, application via RippleMatch</t>
+          <t>Data Engineer II</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Malibu, CA</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/ripplematchinterns/jobs/7417813002</t>
+          <t>New York, NY / Boston, MA</t>
+        </is>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/spotify/359dff96-1818-40b8-a56a-1b6de80726a2</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Truveta</t>
+          <t>brightwheel</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ML Postdoc Researcher - LLMs &amp; Generative AI</t>
+          <t>Director of Sales, Expansion</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/truveta/jobs/4898482004</t>
+          <t>Remote (US Only)</t>
+        </is>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/brightwheel/0627a0f8-cab0-4905-9660-55e8ecf17144</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Box</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Software Engineer, Observability</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Redwood City, CA</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/boxinc/jobs/5614752</t>
+          <t>Remote - United States</t>
+        </is>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/thetrevorproject/b78c5e62-8495-493a-9a0b-6f3681b8c045</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -1184,250 +1279,290 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>https://boards.eu.greenhouse.io/abbyy/jobs/4302613101</t>
+          <t>Remote NA</t>
+        </is>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/aircall/5c1cec11-88fc-4349-9b39-1ca59a806952</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Vonage</t>
+          <t>UpGuard</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Python - Backend Engineer</t>
+          <t>People Partner</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/vonage/jobs/7090195002</t>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/upguard/b42ecb34-bec3-4e20-9c63-12cc076e9677</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Gopuff</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Retail Key Holder, Visalia, #419</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/spacex/jobs/72336960027233696002</t>
+          <t>Visalia, CA</t>
+        </is>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/gopuff/f4dc94a2-f52c-4b57-be2d-c47722a20d00</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Together AI</t>
+          <t>Edpuzzle</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>AI Researcher, NLP and Computer Vision</t>
+          <t>K-12 Sales Representative, Texas</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>San Francisco</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/togetherai/jobs/4188035007</t>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/edpuzzle/907bac57-ad16-4464-b049-65204c38517e</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Isomorphic Labs</t>
+          <t>Gauntlet</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Bioinformatics Engineer</t>
+          <t>Head of Information Security</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>London</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/isomorphiclabs/jobs/5035792004</t>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/gauntlet/41e47437-307c-483e-add4-67e42d5e3b09</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Smartling</t>
+          <t>Varo Bank</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Linguistic Engineer</t>
+          <t>Chief Credit Officer</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/smartling/jobs/5950645</t>
+          <t>Charlotte, NC / Salt Lake City, UT / San Francisco, CA / US Remote</t>
+        </is>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/varomoney/b0c8b3ed-bde2-4610-afdd-c515d2d11866</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>KoBold Metals</t>
+          <t>ABL Space Systems</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Infrastructure Engineer</t>
+          <t>Environmental Test Lab Technician</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Remote</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/koboldmetals/jobs/4400868005</t>
+          <t>El Segundo, California</t>
+        </is>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/ablspacesystems/2cc23e21-1354-40a1-80b4-b5d0ba44e2a2</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Latitude AI</t>
+          <t>Picus</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Software Engineer II, Cloud Services</t>
+          <t>Sales Operations &amp; Analysis Specialist (US)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Palo Alto CA, Pittsburgh PA, Detroit MI</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/latitude/jobs/5848856</t>
+          <t>Ankara, Turkey / Istanbul, Turkey</t>
+        </is>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/picus/8a9f6591-1a06-4d9a-828e-e75094674835</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>InstaDeep</t>
+          <t>JMA Wireless</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Research Engineer</t>
+          <t>Mechanical Engineer (ME1)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>London</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>https://jobs.eu.lever.co/instadeep/dfd57254-147a-40e3-b6fb-efbc557d64a6</t>
+          <t>Plano, Texas</t>
+        </is>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/jmawireless/1d815e9c-2413-4a4c-a949-eb52d8e46bba</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Cars Commerce</t>
+          <t>Qvest.US</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Data Scientist II</t>
+          <t>Administrative Assistant</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>United States, Remote</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/carsdotcom/jobs/5808218</t>
+          <t>Austin, Texas / New York, New York</t>
+        </is>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/qvest.us/f1ab67b8-3129-412c-9076-0dcea44b3382</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fama Technologies Inc.</t>
+          <t>Welocalize</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Junior Machine Learning Engineer</t>
+          <t>Internet Search Coding Expert</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/fama/90a571a3-1cef-4f6b-9ce4-c5c63e8e1604</t>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/welocalize/940d5f1f-5d14-4b93-8640-f29a36a8998a</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Bolster Inc.</t>
+          <t>Toyota Research Institute</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Front-End Engineer</t>
+          <t>Postdoctoral Researcher, Foundation Models for Driving</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Noida</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>https://jobs.lever.co/bolster/f05cab87-0afb-4208-afdc-d6ede35b781e</t>
+          <t>Los Altos, CA</t>
+        </is>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://jobs.lever.co/tri/59485fcd-a84c-4956-983f-1db328766aca</t>
         </is>
       </c>
     </row>

</xml_diff>